<commit_message>
modify action basic logic,all move should extend from action,than do their unique set,create arena2 to test this concept
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A3504\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D_temp\TESTING\RPG_TEST\RPG_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7545" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7545" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="build your team" sheetId="4" r:id="rId4"/>
     <sheet name="Place" sheetId="5" r:id="rId5"/>
     <sheet name="If AI" sheetId="6" r:id="rId6"/>
-    <sheet name="MapConcept" sheetId="7" r:id="rId7"/>
+    <sheet name="Round design" sheetId="8" r:id="rId7"/>
+    <sheet name="MapConcept" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -5822,6 +5823,328 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="圓角矩形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="942975" y="342900"/>
+          <a:ext cx="6296025" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1609725" y="504825"/>
+          <a:ext cx="1381125" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Action collections</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>order by:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>1.priority</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>2.SPD</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1647825" y="1676400"/>
+          <a:ext cx="4210050" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>foreach(Action</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t> act in actions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>){</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t>   if(act.available()){//return available status,if false,</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t>      do_action </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t>   }else{</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t>      show_fail_msg</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t>   }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>	</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>}</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+          </a:br>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="矩形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7648575" y="400050"/>
+          <a:ext cx="6276975" cy="4210050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -6813,6 +7136,89 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="文字方塊 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8362950" y="457200"/>
+          <a:ext cx="4600575" cy="3733800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>I think</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t> maybe use graph structure?if need so complex...</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t>if not so complex,LinkedList and tree might be easiler option</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7185,8 +7591,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>